<commit_message>
scores for ngram(1,3) for two and three level
</commit_message>
<xml_diff>
--- a/research results/Three Level Numbers.xlsx
+++ b/research results/Three Level Numbers.xlsx
@@ -7,15 +7,16 @@
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="LogisticRegression - Obesity" sheetId="1" r:id="rId1"/>
-    <sheet name="Summary" sheetId="2" r:id="rId2"/>
+    <sheet name="SVM - Obesity" sheetId="3" r:id="rId1"/>
+    <sheet name="LogisticRegression - Obesity" sheetId="1" r:id="rId2"/>
+    <sheet name="Summary" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>Min Preprocessing</t>
   </si>
@@ -99,6 +100,9 @@
   </si>
   <si>
     <t>Using LR, one hot encoding, min preprocessing and ngram(1,2)</t>
+  </si>
+  <si>
+    <t>ngram(1,3)</t>
   </si>
 </sst>
 </file>
@@ -189,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -211,6 +215,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C19"/>
+  <dimension ref="A2:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,127 +552,170 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="11">
         <v>94.6</v>
       </c>
-      <c r="C4" s="1">
-        <v>94.6</v>
+      <c r="C4" s="12">
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
-        <v>95.2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>94.8</v>
+      <c r="B5" s="11">
+        <v>94.9</v>
+      </c>
+      <c r="C5" s="11">
+        <v>94.6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
+        <v>94.9</v>
+      </c>
+      <c r="C6" s="11">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="11">
         <v>95</v>
       </c>
-      <c r="C6" s="1">
-        <v>93.5</v>
+      <c r="C7" s="1">
+        <v>94.5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>94.6</v>
-      </c>
-      <c r="C11" s="1">
-        <v>94.2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="11">
-        <v>95</v>
-      </c>
-      <c r="C12" s="1">
-        <v>94.7</v>
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>94.3</v>
+      </c>
+      <c r="C12" s="12">
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="11">
+        <v>94.4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>94.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="1">
-        <v>94.6</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B14" s="4">
+        <v>94.9</v>
+      </c>
+      <c r="C14" s="1">
         <v>93.5</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="11">
+        <v>95</v>
+      </c>
+      <c r="C15" s="11">
+        <v>93.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="1">
-        <v>87.7</v>
-      </c>
-      <c r="C17" s="1">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="1">
-        <v>86.2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="11">
+        <v>93.1</v>
+      </c>
+      <c r="C19" s="11">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="4">
+        <v>94.9</v>
+      </c>
+      <c r="C20" s="11">
+        <v>94.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="1">
-        <v>80.7</v>
-      </c>
-      <c r="C19" s="12">
-        <v>79.7</v>
+      <c r="B21" s="11">
+        <v>94.5</v>
+      </c>
+      <c r="C21" s="11">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="11">
+        <v>94.8</v>
+      </c>
+      <c r="C22" s="11">
+        <v>94.2</v>
       </c>
     </row>
   </sheetData>
@@ -676,6 +725,211 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>94.6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>94.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>95.2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>94.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>95</v>
+      </c>
+      <c r="C6" s="1">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1">
+        <v>94.3</v>
+      </c>
+      <c r="C7" s="1">
+        <v>94.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>94.6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>94.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="11">
+        <v>95</v>
+      </c>
+      <c r="C13" s="1">
+        <v>94.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>94.6</v>
+      </c>
+      <c r="C14" s="1">
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
+        <v>94.3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>94.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>87.7</v>
+      </c>
+      <c r="C19" s="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>86.2</v>
+      </c>
+      <c r="C20" s="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1">
+        <v>80.7</v>
+      </c>
+      <c r="C21" s="12">
+        <v>79.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1">
+        <v>86.7</v>
+      </c>
+      <c r="C22" s="1">
+        <v>81.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>

</xml_diff>